<commit_message>
made new changes to the Report utility class by adding a function that for record table data.
</commit_message>
<xml_diff>
--- a/KeywordDrivenTestPacks/TaskTwo_Automation_one.xlsx
+++ b/KeywordDrivenTestPacks/TaskTwo_Automation_one.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="850" activeTab="1"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="28" r:id="rId1"/>
     <sheet name="AddUser" sheetId="29" r:id="rId2"/>
+    <sheet name="FindNewUser" sheetId="30" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
   <si>
     <t>Path</t>
   </si>
@@ -693,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,38 +950,6 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D18" r:id="rId1"/>
@@ -988,4 +957,68 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>